<commit_message>
added code for crosses and stocks
</commit_message>
<xml_diff>
--- a/data/flymanager_export.xlsx
+++ b/data/flymanager_export.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="food_types" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="transgenesX" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="transgenes4th" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="transgenes3rd" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="activity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="provenances" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="types" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="transgenes2nd" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="users" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="provenances" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="genes3rd" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="genes2nd" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="genes4th" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="users" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="types" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="activity" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="foodtypes" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="genesX" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="admin_Stock" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
@@ -570,7 +570,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec272d</t>
+          <t>66bc3e5ff02388d4a5cb77c0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -661,7 +661,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec272e</t>
+          <t>66bc3e5ff02388d4a5cb77c1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -752,7 +752,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec272f</t>
+          <t>66bc3e5ff02388d4a5cb77c2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -839,7 +839,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2730</t>
+          <t>66bc3e5ff02388d4a5cb77c3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -934,7 +934,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2731</t>
+          <t>66bc3e5ff02388d4a5cb77c4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1029,7 +1029,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2732</t>
+          <t>66bc3e5ff02388d4a5cb77c5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1124,7 +1124,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2733</t>
+          <t>66bc3e5ff02388d4a5cb77c6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1219,7 +1219,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2734</t>
+          <t>66bc3e5ff02388d4a5cb77c7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1314,7 +1314,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2735</t>
+          <t>66bc3e5ff02388d4a5cb77c8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1405,7 +1405,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2736</t>
+          <t>66bc3e5ff02388d4a5cb77c9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2737</t>
+          <t>66bc3e5ff02388d4a5cb77ca</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1579,7 +1579,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2738</t>
+          <t>66bc3e5ff02388d4a5cb77cb</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1666,7 +1666,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2739</t>
+          <t>66bc3e5ff02388d4a5cb77cc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1753,7 +1753,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273a</t>
+          <t>66bc3e5ff02388d4a5cb77cd</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1844,7 +1844,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273b</t>
+          <t>66bc3e5ff02388d4a5cb77ce</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1931,7 +1931,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273c</t>
+          <t>66bc3e5ff02388d4a5cb77cf</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273d</t>
+          <t>66bc3e5ff02388d4a5cb77d0</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2105,7 +2105,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273e</t>
+          <t>66bc3e5ff02388d4a5cb77d1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2196,7 +2196,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec273f</t>
+          <t>66bc3e5ff02388d4a5cb77d2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2287,7 +2287,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2740</t>
+          <t>66bc3e5ff02388d4a5cb77d3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2741</t>
+          <t>66bc3e5ff02388d4a5cb77d4</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2469,7 +2469,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2742</t>
+          <t>66bc3e5ff02388d4a5cb77d5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2560,7 +2560,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2743</t>
+          <t>66bc3e5ff02388d4a5cb77d6</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2651,7 +2651,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2744</t>
+          <t>66bc3e5ff02388d4a5cb77d7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2742,7 +2742,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2745</t>
+          <t>66bc3e5ff02388d4a5cb77d8</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2837,7 +2837,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2746</t>
+          <t>66bc3e5ff02388d4a5cb77d9</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>w[1118]; P{y[+t7.7] w[+mC]=20XUAS-IVS-CsChrimson.mVenus}attP18; ; ;</t>
+          <t>w[1118] P{y[+t7.7] w[+mC]=20XUAS-IVS-CsChrimson.mVenus}attP18; ; ;</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2928,7 +2928,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2747</t>
+          <t>66bc3e5ff02388d4a5cb77da</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>w[1118]; P{y[+t7.7] w[+mC]=20XUAS-IVS-CsChrimson.mVenus}attP18; ; ;</t>
+          <t>w[1118] P{y[+t7.7] w[+mC]=20XUAS-IVS-CsChrimson.mVenus}attP18; ; ;</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3019,7 +3019,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2748</t>
+          <t>66bc3e5ff02388d4a5cb77db</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2749</t>
+          <t>66bc3e5ff02388d4a5cb77dc</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3201,7 +3201,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec274a</t>
+          <t>66bc3e5ff02388d4a5cb77dd</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3300,7 +3300,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec274b</t>
+          <t>66bc3e5ff02388d4a5cb77de</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3461,7 +3461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3477,24 +3477,24 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>username</t>
+          <t>Username</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>Password</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>activity</t>
+          <t>Initials</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>66bc27ff4d3dc02fb3ec2723</t>
+          <t>66bc3e5ff02388d4a5cb77b5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3504,210 +3504,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-29 14:17:37</t>
+          <t>74c43abb6c</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>User added</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2724</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-08-09 14:02:13</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Generated labels for 2 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2725</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-08-09 14:07:33</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Generated labels for 2 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2726</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2024-08-09 16:06:54</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Generated labels for 16 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2727</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2024-08-12 09:42:42</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Generated labels for 3 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2728</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2024-08-12 09:47:04</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Generated labels for 16 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2729</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2024-08-12 14:47:58</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Generated labels for 16 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec272a</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2024-08-12 17:33:52</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Generated labels for 10 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec272b</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2024-08-12 17:35:51</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Generated labels for 10 stocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec272c</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2024-08-12 17:39:04</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Generated labels for 10 stocks</t>
+          <t>RM</t>
         </is>
       </c>
     </row>
@@ -3740,14 +3542,257 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77b6</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-07-29 14:17:37</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>User added</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77b7</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-08-09 14:02:13</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Generated labels for 2 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77b8</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-08-09 14:07:33</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Generated labels for 2 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77b9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-08-09 16:06:54</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Generated labels for 16 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77ba</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-08-12 09:42:42</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Generated labels for 3 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77bb</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-08-12 09:47:04</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Generated labels for 16 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77bc</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-08-12 14:47:58</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Generated labels for 16 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77bd</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-08-12 17:33:52</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Generated labels for 10 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77be</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-08-12 17:35:51</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Generated labels for 10 stocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>66bc3e5ff02388d4a5cb77bf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-08-12 17:39:04</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Generated labels for 10 stocks</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3776,59 +3821,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Initials</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>66bc27ff4d3dc02fb3ec2722</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>74c43abb6c</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>RM</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>